<commit_message>
Better architecture diagram and fix a FAQ entry. (#455)
</commit_message>
<xml_diff>
--- a/docs/docs/images/arch-diagram.xlsx
+++ b/docs/docs/images/arch-diagram.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Corda/conclave/docs/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Corda/conclave/docs/docs/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727A62A4-B24E-384E-9DB7-1E5A07549407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADBC110-4EFB-3743-98DE-63FF9E303D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-7340" windowWidth="51200" windowHeight="28340" xr2:uid="{2ED672D7-C865-D444-BDEA-C0A5C51D3721}"/>
   </bookViews>
@@ -308,16 +308,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>732953</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>111464</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>101329</xdr:rowOff>
+      <xdr:rowOff>91196</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>91199</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>145238</xdr:rowOff>
+      <xdr:colOff>6755</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>179014</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -332,8 +332,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="2381251" y="506648"/>
-          <a:ext cx="1830693" cy="246569"/>
+          <a:off x="3408060" y="496515"/>
+          <a:ext cx="719440" cy="695797"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1018,7 +1018,7 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="376" zoomScaleNormal="376" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>